<commit_message>
Término da atividade 'Prova 2des' - LIMA
</commit_message>
<xml_diff>
--- a/FPOO/Java/aula2_verde/workspace/Alunos/excel/Alunos1.xlsx
+++ b/FPOO/Java/aula2_verde/workspace/Alunos/excel/Alunos1.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25813"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/645ba0ac008cf914/Área de Trabalho/SENAI/Diretorios/desenvolvimento-de-sistemas/FPOO/Java/aula2_verde/workspace/Alunos/excel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D694A03-9EE7-4CF1-94DD-33791AF9C12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{30C2B299-9EB6-4C87-B6F9-F5E0FD10DD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B16FA8E6-ED7B-4668-912F-C9751915C7BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B16FA8E6-ED7B-4668-912F-C9751915C7BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +19,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -107,16 +106,16 @@
     <t>Idoso</t>
   </si>
   <si>
-    <t>&gt;0 &lt;=13</t>
-  </si>
-  <si>
-    <t>&gt;13 &lt;=20</t>
-  </si>
-  <si>
-    <t>&gt;20 &lt;=60</t>
-  </si>
-  <si>
-    <t>&gt;60</t>
+    <t>&gt; 0 &lt;= 13</t>
+  </si>
+  <si>
+    <t>&gt;13 &lt;= 20</t>
+  </si>
+  <si>
+    <t>&gt; 20 &lt;= 60</t>
+  </si>
+  <si>
+    <t>&gt; 60</t>
   </si>
 </sst>
 </file>
@@ -508,7 +507,7 @@
   <dimension ref="F1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>